<commit_message>
hoja de excel con valores correspondientes
</commit_message>
<xml_diff>
--- a/respuestas a encuesta.xlsx
+++ b/respuestas a encuesta.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="39">
   <si>
     <t>De acuerdo</t>
   </si>
@@ -133,6 +133,15 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Tiempo en la empresa</t>
+  </si>
+  <si>
+    <t>Respuesta</t>
+  </si>
 </sst>
 </file>
 
@@ -235,861 +244,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$D$70:$D$71</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Ingeniería en Sistemas Computacionales</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ingeniería en Cómputación Inteligente</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$E$70:$E$71</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6F26-498F-A86A-4FA8B93F75F2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="527175096"/>
-        <c:axId val="527175424"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="527175096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527175424"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="527175424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527175096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Gráfico 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4BA6580-87C4-4F21-AC84-AC966B66C09F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1389,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCE11A1-7572-459E-B136-9E51D6E6530F}">
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70:F71"/>
+    <sheetView tabSelected="1" topLeftCell="C141" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157:F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,8 +554,17 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="128.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4503,6 +3666,15 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D69" t="s">
         <v>26</v>
       </c>
@@ -4514,12 +3686,16 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>28</v>
+      <c r="A70" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B70">
-        <f>COUNTIF(D2:D67, "&lt;=21")</f>
-        <v>10</v>
+        <f>COUNTIF(E2:E67, "1 - 3 Meses")</f>
+        <v>15</v>
+      </c>
+      <c r="C70">
+        <f>B70*100/B74</f>
+        <v>22.727272727272727</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>4</v>
@@ -4534,12 +3710,16 @@
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>29</v>
+      <c r="A71" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B71">
-        <f>COUNTIF(D2:D67, "&lt;=24") - B70</f>
-        <v>37</v>
+        <f>COUNTIF(E2:E67, "3 - 6 Meses")</f>
+        <v>12</v>
+      </c>
+      <c r="C71">
+        <f>B71*100/B74</f>
+        <v>18.181818181818183</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>10</v>
@@ -4554,12 +3734,16 @@
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>30</v>
+      <c r="A72" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B72">
-        <f>COUNTIF(D2:D67, "&lt;=27") - B71 - B70</f>
-        <v>16</v>
+        <f>COUNTIF(E2:E67, "6 Meses - 1 Año")</f>
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <f>B72*100/B74</f>
+        <v>12.121212121212121</v>
       </c>
       <c r="D72" t="s">
         <v>35</v>
@@ -4574,32 +3758,1088 @@
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <f>COUNTIF(E2:E67, "Más de 1 Año")</f>
         <v>31</v>
       </c>
-      <c r="B73">
-        <f>COUNTIF(D2:D67, "&lt;=30") - B72 - B71 - B70</f>
+      <c r="C73">
+        <f>B73*100/B74</f>
+        <v>46.969696969696969</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <f>SUM(B70:B73)</f>
+        <v>66</v>
+      </c>
+      <c r="C74">
+        <f>SUM(C70:C73)</f>
+        <v>100</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <f>COUNTIF(D2:D67, "&lt;=21")</f>
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <f>B76*100/B81</f>
+        <v>15.151515151515152</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <f>COUNTIF(N2:N67, "Totalmente de acuerdo")</f>
+        <v>10</v>
+      </c>
+      <c r="G76">
+        <f>F76*100/66</f>
+        <v>15.151515151515152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77">
+        <f>COUNTIF(D2:D67, "&lt;=24") - B76</f>
+        <v>37</v>
+      </c>
+      <c r="C77">
+        <f>B77*100/B81</f>
+        <v>56.060606060606062</v>
+      </c>
+      <c r="E77" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f>COUNTIF(N2:N67, "De acuerdo")</f>
+        <v>24</v>
+      </c>
+      <c r="G77">
+        <f t="shared" ref="G77:G80" si="0">F77*100/66</f>
+        <v>36.363636363636367</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78">
+        <f>COUNTIF(D2:D67, "&lt;=27") - B77 - B76</f>
+        <v>16</v>
+      </c>
+      <c r="C78">
+        <f>B78*100/B81</f>
+        <v>24.242424242424242</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78">
+        <f>COUNTIF(N2:N67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>15</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="0"/>
+        <v>22.727272727272727</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79">
+        <f>COUNTIF(D2:D67, "&lt;=30") - B78 - B77 - B76</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="C79">
+        <f>B79*100/B81</f>
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <f>COUNTIF(N2:N67, "En desacuerdo")</f>
+        <v>11</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B74">
+      <c r="B80">
         <f>COUNTIF(D2:D67, "&gt;30")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B75">
-        <f>SUM(B70:B74)</f>
+      <c r="C80">
+        <f>B80*100/B81</f>
+        <v>1.5151515151515151</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80">
+        <f>COUNTIF(N2:N67, "Totalmente en desacuerdo")</f>
+        <v>6</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81">
+        <f>SUM(B76:B80)</f>
         <v>66</v>
+      </c>
+      <c r="C81">
+        <f>SUM(C76:C80)</f>
+        <v>100.00000000000001</v>
+      </c>
+      <c r="E81" t="s">
+        <v>35</v>
+      </c>
+      <c r="F81">
+        <f>SUM(F76:F80)</f>
+        <v>66</v>
+      </c>
+      <c r="G81">
+        <f>SUM(G76:G80)</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E83" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" t="s">
+        <v>33</v>
+      </c>
+      <c r="G84" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <f>COUNTIF(C2:C67, "Hombre")</f>
+        <v>42</v>
+      </c>
+      <c r="C85">
+        <f>B85*100/B87</f>
+        <v>63.636363636363633</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <f>COUNTIF(O2:O67, "Totalmente de acuerdo")</f>
+        <v>15</v>
+      </c>
+      <c r="G85">
+        <f>F85*100/66</f>
+        <v>22.727272727272727</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86">
+        <f>COUNTIF(C2:C67, "Mujer")</f>
+        <v>24</v>
+      </c>
+      <c r="C86">
+        <f>B86*100/B87</f>
+        <v>36.363636363636367</v>
+      </c>
+      <c r="E86" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <f>COUNTIF(O2:O67, "De acuerdo")</f>
+        <v>25</v>
+      </c>
+      <c r="G86">
+        <f t="shared" ref="G86:G89" si="1">F86*100/66</f>
+        <v>37.878787878787875</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87">
+        <f>SUM(B85:B86)</f>
+        <v>66</v>
+      </c>
+      <c r="C87">
+        <f>SUM(C85:C86)</f>
+        <v>100</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87">
+        <f>COUNTIF(O2:O67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>16</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>24.242424242424242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88">
+        <f>COUNTIF(O2:O67, "En desacuerdo")</f>
+        <v>4</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="1"/>
+        <v>6.0606060606060606</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89">
+        <f>COUNTIF(O2:O67, "Totalmente en desacuerdo")</f>
+        <v>6</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>35</v>
+      </c>
+      <c r="F90">
+        <f>SUM(F85:F89)</f>
+        <v>66</v>
+      </c>
+      <c r="G90">
+        <f>SUM(G85:G89)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" t="s">
+        <v>33</v>
+      </c>
+      <c r="G93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <f>COUNTIF(L2:L67, "Totalmente de acuerdo")</f>
+        <v>20</v>
+      </c>
+      <c r="G94">
+        <f>F94*100/66</f>
+        <v>30.303030303030305</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <f>COUNTIF(L2:L67, "De acuerdo")</f>
+        <v>19</v>
+      </c>
+      <c r="G95">
+        <f t="shared" ref="G95:G98" si="2">F95*100/66</f>
+        <v>28.787878787878789</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <f>COUNTIF(L2:L67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>12</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="2"/>
+        <v>18.181818181818183</v>
+      </c>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97">
+        <f>COUNTIF(L2:L67, "En desacuerdo")</f>
+        <v>7</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="2"/>
+        <v>10.606060606060606</v>
+      </c>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98">
+        <f>COUNTIF(L2:L67, "Totalmente en desacuerdo")</f>
+        <v>8</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="2"/>
+        <v>12.121212121212121</v>
+      </c>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>35</v>
+      </c>
+      <c r="F99">
+        <f>SUM(F94:F98)</f>
+        <v>66</v>
+      </c>
+      <c r="G99">
+        <f>SUM(G94:G98)</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>38</v>
+      </c>
+      <c r="F102" t="s">
+        <v>33</v>
+      </c>
+      <c r="G102" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <f>COUNTIF(G2:G67, "Totalmente de acuerdo")</f>
+        <v>27</v>
+      </c>
+      <c r="G103">
+        <f>F103*100/66</f>
+        <v>40.909090909090907</v>
+      </c>
+    </row>
+    <row r="104" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <f>COUNTIF(G2:G67, "De acuerdo")</f>
+        <v>31</v>
+      </c>
+      <c r="G104">
+        <f t="shared" ref="G104:G107" si="3">F104*100/66</f>
+        <v>46.969696969696969</v>
+      </c>
+    </row>
+    <row r="105" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105">
+        <f>COUNTIF(G2:G67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>3</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="3"/>
+        <v>4.5454545454545459</v>
+      </c>
+    </row>
+    <row r="106" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106">
+        <f>COUNTIF(G2:G67, "En desacuerdo")</f>
+        <v>1</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="3"/>
+        <v>1.5151515151515151</v>
+      </c>
+    </row>
+    <row r="107" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107">
+        <f>COUNTIF(G2:G67, "Totalmente en desacuerdo")</f>
+        <v>4</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="3"/>
+        <v>6.0606060606060606</v>
+      </c>
+    </row>
+    <row r="108" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>35</v>
+      </c>
+      <c r="F108">
+        <f>SUM(F103:F107)</f>
+        <v>66</v>
+      </c>
+      <c r="G108">
+        <f>SUM(G103:G107)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>38</v>
+      </c>
+      <c r="F111" t="s">
+        <v>33</v>
+      </c>
+      <c r="G111" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <f>COUNTIF(F2:F67, "Totalmente de acuerdo")</f>
+        <v>26</v>
+      </c>
+      <c r="G112">
+        <f>F112*100/66</f>
+        <v>39.393939393939391</v>
+      </c>
+    </row>
+    <row r="113" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <f>COUNTIF(F2:F67, "De acuerdo")</f>
+        <v>23</v>
+      </c>
+      <c r="G113">
+        <f t="shared" ref="G113:G116" si="4">F113*100/66</f>
+        <v>34.848484848484851</v>
+      </c>
+    </row>
+    <row r="114" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114">
+        <f>COUNTIF(F2:F67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>14</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="4"/>
+        <v>21.212121212121211</v>
+      </c>
+    </row>
+    <row r="115" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115">
+        <f>COUNTIF(F2:F67, "En desacuerdo")</f>
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="4"/>
+        <v>4.5454545454545459</v>
+      </c>
+    </row>
+    <row r="116" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116">
+        <f>COUNTIF(F2:F67, "Totalmente en desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>35</v>
+      </c>
+      <c r="F117">
+        <f>SUM(F112:F116)</f>
+        <v>66</v>
+      </c>
+      <c r="G117">
+        <f>SUM(G112:G116)</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E119" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>38</v>
+      </c>
+      <c r="F120" t="s">
+        <v>33</v>
+      </c>
+      <c r="G120" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <f>COUNTIF(I2:I67, "Totalmente de acuerdo")</f>
+        <v>13</v>
+      </c>
+      <c r="G121">
+        <f>F121*100/66</f>
+        <v>19.696969696969695</v>
+      </c>
+    </row>
+    <row r="122" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E122" t="s">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <f>COUNTIF(I2:I67, "De acuerdo")</f>
+        <v>23</v>
+      </c>
+      <c r="G122">
+        <f t="shared" ref="G122:G125" si="5">F122*100/66</f>
+        <v>34.848484848484851</v>
+      </c>
+    </row>
+    <row r="123" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F123">
+        <f>COUNTIF(I2:I67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>19</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="5"/>
+        <v>28.787878787878789</v>
+      </c>
+    </row>
+    <row r="124" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124">
+        <f>COUNTIF(I2:I67, "En desacuerdo")</f>
+        <v>5</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="5"/>
+        <v>7.5757575757575761</v>
+      </c>
+    </row>
+    <row r="125" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125">
+        <f>COUNTIF(I2:I67, "Totalmente en desacuerdo")</f>
+        <v>6</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="5"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="126" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>35</v>
+      </c>
+      <c r="F126">
+        <f>SUM(F121:F125)</f>
+        <v>66</v>
+      </c>
+      <c r="G126">
+        <f>SUM(G121:G125)</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" t="s">
+        <v>33</v>
+      </c>
+      <c r="G129" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <f>COUNTIF(H2:H67, "Totalmente de acuerdo")</f>
+        <v>17</v>
+      </c>
+      <c r="G130">
+        <f>F130*100/66</f>
+        <v>25.757575757575758</v>
+      </c>
+    </row>
+    <row r="131" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <f>COUNTIF(H2:H67, "De acuerdo")</f>
+        <v>19</v>
+      </c>
+      <c r="G131">
+        <f t="shared" ref="G131:G134" si="6">F131*100/66</f>
+        <v>28.787878787878789</v>
+      </c>
+    </row>
+    <row r="132" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132">
+        <f>COUNTIF(H2:H67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>20</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="6"/>
+        <v>30.303030303030305</v>
+      </c>
+    </row>
+    <row r="133" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133">
+        <f>COUNTIF(H2:H67, "En desacuerdo")</f>
+        <v>5</v>
+      </c>
+      <c r="G133">
+        <f t="shared" si="6"/>
+        <v>7.5757575757575761</v>
+      </c>
+    </row>
+    <row r="134" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134">
+        <f>COUNTIF(H2:H67, "Totalmente en desacuerdo")</f>
+        <v>5</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="6"/>
+        <v>7.5757575757575761</v>
+      </c>
+    </row>
+    <row r="135" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>35</v>
+      </c>
+      <c r="F135">
+        <f>SUM(F130:F134)</f>
+        <v>66</v>
+      </c>
+      <c r="G135">
+        <f>SUM(G130:G134)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="138" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>38</v>
+      </c>
+      <c r="F138" t="s">
+        <v>33</v>
+      </c>
+      <c r="G138" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="139" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <f>COUNTIF(J2:J67, "Totalmente de acuerdo")</f>
+        <v>24</v>
+      </c>
+      <c r="G139">
+        <f>F139*100/66</f>
+        <v>36.363636363636367</v>
+      </c>
+    </row>
+    <row r="140" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <f>COUNTIF(J2:J67, "De acuerdo")</f>
+        <v>22</v>
+      </c>
+      <c r="G140">
+        <f t="shared" ref="G140:G143" si="7">F140*100/66</f>
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="141" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E141" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F141">
+        <f>COUNTIF(J2:J67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>16</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="7"/>
+        <v>24.242424242424242</v>
+      </c>
+    </row>
+    <row r="142" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142">
+        <f>COUNTIF(J2:J67, "En desacuerdo")</f>
+        <v>4</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="7"/>
+        <v>6.0606060606060606</v>
+      </c>
+    </row>
+    <row r="143" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143">
+        <f>COUNTIF(J2:J67, "Totalmente en desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>35</v>
+      </c>
+      <c r="F144">
+        <f>SUM(F139:F143)</f>
+        <v>66</v>
+      </c>
+      <c r="G144">
+        <f>SUM(G139:G143)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="146" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>38</v>
+      </c>
+      <c r="F147" t="s">
+        <v>33</v>
+      </c>
+      <c r="G147" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="148" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <f>COUNTIF(K2:K67, "Totalmente de acuerdo")</f>
+        <v>15</v>
+      </c>
+      <c r="G148">
+        <f>F148*100/66</f>
+        <v>22.727272727272727</v>
+      </c>
+    </row>
+    <row r="149" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <f>COUNTIF(K2:K67, "De acuerdo")</f>
+        <v>24</v>
+      </c>
+      <c r="G149">
+        <f t="shared" ref="G149:G152" si="8">F149*100/66</f>
+        <v>36.363636363636367</v>
+      </c>
+    </row>
+    <row r="150" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F150">
+        <f>COUNTIF(K2:K67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>17</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="8"/>
+        <v>25.757575757575758</v>
+      </c>
+    </row>
+    <row r="151" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>8</v>
+      </c>
+      <c r="F151">
+        <f>COUNTIF(K2:K67, "En desacuerdo")</f>
+        <v>10</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="8"/>
+        <v>15.151515151515152</v>
+      </c>
+    </row>
+    <row r="152" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E152" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152">
+        <f>COUNTIF(K2:K67, "Totalmente en desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E153" t="s">
+        <v>35</v>
+      </c>
+      <c r="F153">
+        <f>SUM(F148:F152)</f>
+        <v>66</v>
+      </c>
+      <c r="G153">
+        <f>SUM(G148:G152)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E155" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E156" t="s">
+        <v>38</v>
+      </c>
+      <c r="F156" t="s">
+        <v>33</v>
+      </c>
+      <c r="G156" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="157" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E157" t="s">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <f>COUNTIF(M2:M67, "Totalmente de acuerdo")</f>
+        <v>23</v>
+      </c>
+      <c r="G157">
+        <f>F157*100/66</f>
+        <v>34.848484848484851</v>
+      </c>
+    </row>
+    <row r="158" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E158" t="s">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <f>COUNTIF(M2:M67, "De acuerdo")</f>
+        <v>28</v>
+      </c>
+      <c r="G158">
+        <f t="shared" ref="G158:G161" si="9">F158*100/66</f>
+        <v>42.424242424242422</v>
+      </c>
+    </row>
+    <row r="159" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E159" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F159">
+        <f>COUNTIF(M2:M67, "Ni de acuerdo ni en desacuerdo")</f>
+        <v>11</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="9"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="160" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E160" t="s">
+        <v>8</v>
+      </c>
+      <c r="F160">
+        <f>COUNTIF(M2:M67, "En desacuerdo")</f>
+        <v>4</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="9"/>
+        <v>6.0606060606060606</v>
+      </c>
+    </row>
+    <row r="161" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E161" t="s">
+        <v>11</v>
+      </c>
+      <c r="F161">
+        <f>COUNTIF(M2:M67, "Totalmente en desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E162" t="s">
+        <v>35</v>
+      </c>
+      <c r="F162">
+        <f>SUM(F157:F161)</f>
+        <v>66</v>
+      </c>
+      <c r="G162">
+        <f>SUM(G157:G161)</f>
+        <v>100.00000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>